<commit_message>
update data_manifest and name_matching file
</commit_message>
<xml_diff>
--- a/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
+++ b/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24860" windowHeight="16740"/>
+    <workbookView windowHeight="16740"/>
   </bookViews>
   <sheets>
     <sheet name="Data - Inclusive Digital Data R" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411">
   <si>
     <t>Indicator</t>
   </si>
@@ -229,7 +229,7 @@
     <t>International Energy Agency / Global Competitiveness Index</t>
   </si>
   <si>
-    <t>elec_supply_quality</t>
+    <t>elect_supply_quality</t>
   </si>
   <si>
     <t>http://reports.weforum.org/global-competitiveness-report-2019/downloads/</t>
@@ -244,7 +244,7 @@
     <t>Electrical Distribution Grid Maps</t>
   </si>
   <si>
-    <t>elec_dist_gride_maps</t>
+    <t>elect_dist_grid_maps</t>
   </si>
   <si>
     <t>https://data.humdata.org/dataset/electricaldistributiongridmaps</t>
@@ -256,7 +256,7 @@
     <t>Telecommunication Infrastructure Index (TII)</t>
   </si>
   <si>
-    <t>tii</t>
+    <t>tii_countries</t>
   </si>
   <si>
     <t>Arithmetic average composite of five indicators: (i) estimated internet users per 100 inhabitants; (ii) number of main fixed telephone lines per 100 inhabitants; (iii) number of mobile subscribers per 100 inhabitants; (iv) number of wireless broadband subscriptions per 100 inhabitants; and (v) number of fixed broadband subscriptions per 100 inhabitants.</t>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>GIGA</t>
+  </si>
+  <si>
+    <t>schools_w_internet</t>
   </si>
   <si>
     <t>https://projectconnect.unicef.io/</t>
@@ -522,7 +525,7 @@
     <t>DESA</t>
   </si>
   <si>
-    <t>E-Government Index, E-Participation Index, Online Service Index, Human Capital Index, Telecommunication Infrastructure Index 2020.csv</t>
+    <t>gov_osi</t>
   </si>
   <si>
     <t>To arrive at a set of Online Service Index (OSI) values for 2016, a total of 111 researchers, including UN experts and online United Nations Volunteers (UNVs) from over 60 countries with coverage of 66 languages assessed each country’s national website in the native language, including the national portal, e-services portal and e-participation portal, as well as the websites of the related ministries of education, labour, social services, health, finance and environment as applicable.</t>
@@ -541,6 +544,9 @@
   </si>
   <si>
     <t xml:space="preserve">UN </t>
+  </si>
+  <si>
+    <t>countries_epi</t>
   </si>
   <si>
     <t>The e-participation index (EPI) is derived as a supplementary index to the UN E-Government Survey. It extends the dimension of the Survey by focusing on the use of online services to facilitate provision of information by governments to citizens (“e-information sharing”), interaction with stakeholders (“e-consultation”) and engagement in decision-making processes</t>
@@ -1255,10 +1261,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -1373,6 +1379,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1381,16 +1409,47 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1405,7 +1464,43 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1419,101 +1514,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1561,13 +1567,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1579,109 +1597,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1699,13 +1615,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1717,25 +1735,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1754,56 +1760,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1833,6 +1789,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1846,153 +1817,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2096,9 +2102,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2359,17 +2362,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y1132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2468,7 +2471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="2" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -2500,7 +2503,7 @@
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="130" hidden="1" customHeight="1" spans="1:25">
+    <row r="3" s="1" customFormat="1" ht="130" customHeight="1" spans="1:25">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -2535,7 +2538,7 @@
       <c r="X3" s="7"/>
       <c r="Y3" s="31"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="4" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -2569,7 +2572,7 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
     </row>
-    <row r="5" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="5" customFormat="1" customHeight="1" spans="1:24">
       <c r="A5" s="9" t="s">
         <v>33</v>
       </c>
@@ -2607,7 +2610,7 @@
       <c r="W5" s="11"/>
       <c r="X5" s="11"/>
     </row>
-    <row r="6" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="6" customFormat="1" customHeight="1" spans="1:24">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
@@ -2645,7 +2648,7 @@
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="7" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A7" s="7" t="s">
         <v>39</v>
       </c>
@@ -2685,7 +2688,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="8" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
@@ -2725,7 +2728,7 @@
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
     </row>
-    <row r="9" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="9" customFormat="1" customHeight="1" spans="1:24">
       <c r="A9" s="9" t="s">
         <v>46</v>
       </c>
@@ -2763,7 +2766,7 @@
       <c r="W9" s="11"/>
       <c r="X9" s="11"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="10" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A10" s="7" t="s">
         <v>47</v>
       </c>
@@ -2803,7 +2806,7 @@
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="11" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A11" s="7" t="s">
         <v>51</v>
       </c>
@@ -2843,7 +2846,7 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="12" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A12" s="7" t="s">
         <v>54</v>
       </c>
@@ -2883,7 +2886,7 @@
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="13" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -2923,7 +2926,7 @@
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
     </row>
-    <row r="14" s="2" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="14" s="2" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A14" s="12" t="s">
         <v>58</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="15" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A15" s="7" t="s">
         <v>63</v>
       </c>
@@ -3002,7 +3005,7 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="16" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -3040,7 +3043,7 @@
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="17" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A17" s="7" t="s">
         <v>68</v>
       </c>
@@ -3082,7 +3085,7 @@
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
     </row>
-    <row r="18" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="18" customFormat="1" customHeight="1" spans="1:24">
       <c r="A18" s="7" t="s">
         <v>73</v>
       </c>
@@ -3116,7 +3119,7 @@
       <c r="W18" s="11"/>
       <c r="X18" s="11"/>
     </row>
-    <row r="19" s="3" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="19" s="3" customFormat="1" customHeight="1" spans="1:24">
       <c r="A19" s="9" t="s">
         <v>74</v>
       </c>
@@ -3156,7 +3159,7 @@
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
     </row>
-    <row r="20" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="20" customFormat="1" customHeight="1" spans="1:24">
       <c r="A20" s="9" t="s">
         <v>77</v>
       </c>
@@ -3194,7 +3197,7 @@
       <c r="W20" s="11"/>
       <c r="X20" s="11"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="21" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A21" s="7" t="s">
         <v>78</v>
       </c>
@@ -3246,7 +3249,7 @@
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
     </row>
-    <row r="22" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="22" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A22" s="7" t="s">
         <v>83</v>
       </c>
@@ -3286,7 +3289,7 @@
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="39" hidden="1" customHeight="1" spans="1:24">
+    <row r="23" s="1" customFormat="1" ht="39" customHeight="1" spans="1:24">
       <c r="A23" s="7" t="s">
         <v>87</v>
       </c>
@@ -3324,7 +3327,7 @@
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
     </row>
-    <row r="24" s="1" customFormat="1" ht="204" hidden="1" customHeight="1" spans="1:24">
+    <row r="24" s="1" customFormat="1" ht="204" customHeight="1" spans="1:24">
       <c r="A24" s="7" t="s">
         <v>89</v>
       </c>
@@ -3370,7 +3373,7 @@
       </c>
       <c r="X24" s="7"/>
     </row>
-    <row r="25" s="1" customFormat="1" ht="154" hidden="1" customHeight="1" spans="1:24">
+    <row r="25" s="1" customFormat="1" ht="154" customHeight="1" spans="1:24">
       <c r="A25" s="7" t="s">
         <v>96</v>
       </c>
@@ -3416,7 +3419,7 @@
       </c>
       <c r="X25" s="7"/>
     </row>
-    <row r="26" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="26" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A26" s="7" t="s">
         <v>97</v>
       </c>
@@ -3454,7 +3457,7 @@
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="27" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A27" s="7" t="s">
         <v>99</v>
       </c>
@@ -3492,7 +3495,7 @@
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
     </row>
-    <row r="28" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="28" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A28" s="7" t="s">
         <v>101</v>
       </c>
@@ -3530,7 +3533,7 @@
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="29" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A29" s="7" t="s">
         <v>104</v>
       </c>
@@ -3568,7 +3571,7 @@
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="30" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A30" s="7" t="s">
         <v>105</v>
       </c>
@@ -3606,7 +3609,7 @@
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
     </row>
-    <row r="31" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="31" customFormat="1" customHeight="1" spans="1:24">
       <c r="A31" s="9" t="s">
         <v>106</v>
       </c>
@@ -3644,7 +3647,7 @@
       <c r="W31" s="11"/>
       <c r="X31" s="11"/>
     </row>
-    <row r="32" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="32" customFormat="1" customHeight="1" spans="1:24">
       <c r="A32" s="9" t="s">
         <v>107</v>
       </c>
@@ -3682,7 +3685,7 @@
       <c r="W32" s="11"/>
       <c r="X32" s="11"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="33" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A33" s="7" t="s">
         <v>108</v>
       </c>
@@ -3718,7 +3721,7 @@
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="34" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A34" s="7" t="s">
         <v>109</v>
       </c>
@@ -3794,7 +3797,7 @@
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
     </row>
-    <row r="36" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="36" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A36" s="7" t="s">
         <v>113</v>
       </c>
@@ -3856,11 +3859,13 @@
       <c r="F37" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G37" s="7"/>
+      <c r="G37" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
@@ -3879,7 +3884,7 @@
     </row>
     <row r="38" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A38" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="7" t="s">
@@ -3889,18 +3894,18 @@
         <v>36</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F38" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
@@ -3917,9 +3922,9 @@
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
     </row>
-    <row r="39" s="2" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="39" s="2" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A39" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="12" t="s">
@@ -3935,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
@@ -3955,12 +3960,12 @@
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
       <c r="Y39" s="32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A40" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7" t="s">
@@ -3970,18 +3975,18 @@
         <v>36</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F40" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
@@ -3997,29 +4002,29 @@
       <c r="T40" s="7"/>
       <c r="U40" s="7"/>
       <c r="V40" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="W40" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X40" s="7"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="41" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A41" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F41" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="20"/>
@@ -4039,25 +4044,25 @@
       <c r="X41" s="7"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="42" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A42" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F42" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
@@ -4079,35 +4084,35 @@
       <c r="W42" s="7"/>
       <c r="X42" s="7"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="43" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A43" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B43" s="16"/>
       <c r="C43" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F43" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
       <c r="M43" s="22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
@@ -4121,35 +4126,35 @@
       <c r="W43" s="7"/>
       <c r="X43" s="7"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="44" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A44" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F44" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
       <c r="J44" s="20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
       <c r="M44" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
@@ -4163,9 +4168,9 @@
       <c r="W44" s="7"/>
       <c r="X44" s="7"/>
     </row>
-    <row r="45" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="45" customFormat="1" customHeight="1" spans="1:24">
       <c r="A45" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>34</v>
@@ -4174,7 +4179,7 @@
         <v>35</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>37</v>
@@ -4201,9 +4206,9 @@
       <c r="W45" s="11"/>
       <c r="X45" s="11"/>
     </row>
-    <row r="46" customFormat="1" hidden="1" customHeight="1" spans="1:24">
+    <row r="46" customFormat="1" customHeight="1" spans="1:24">
       <c r="A46" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>34</v>
@@ -4212,7 +4217,7 @@
         <v>35</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>37</v>
@@ -4239,19 +4244,19 @@
       <c r="W46" s="11"/>
       <c r="X46" s="11"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="47" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A47" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F47" s="7" t="b">
         <v>0</v>
@@ -4277,23 +4282,23 @@
     </row>
     <row r="48" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A48" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F48" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -4315,23 +4320,23 @@
     </row>
     <row r="49" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A49" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F49" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
@@ -4353,23 +4358,23 @@
     </row>
     <row r="50" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A50" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F50" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -4391,23 +4396,23 @@
     </row>
     <row r="51" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A51" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F51" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -4429,17 +4434,17 @@
     </row>
     <row r="52" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A52" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F52" s="7" t="b">
         <v>0</v>
@@ -4448,7 +4453,7 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="20" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
@@ -4465,32 +4470,32 @@
       <c r="W52" s="7"/>
       <c r="X52" s="7"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="53" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A53" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F53" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="G53" s="5" t="s">
-        <v>167</v>
+      <c r="G53" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K53" s="7"/>
       <c r="L53" s="30">
@@ -4507,7 +4512,7 @@
       </c>
       <c r="P53" s="7"/>
       <c r="Q53" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="R53" s="7"/>
       <c r="S53" s="7"/>
@@ -4519,31 +4524,31 @@
       <c r="W53" s="7"/>
       <c r="X53" s="7"/>
       <c r="Y53" s="33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A54" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F54" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
@@ -4570,21 +4575,21 @@
       <c r="W54" s="7"/>
       <c r="X54" s="7"/>
       <c r="Y54" s="33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" customFormat="1" ht="48" hidden="1" spans="1:24">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" customFormat="1" ht="48" spans="1:24">
       <c r="A55" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>37</v>
@@ -4611,18 +4616,18 @@
       <c r="W55" s="11"/>
       <c r="X55" s="11"/>
     </row>
-    <row r="56" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="56" customFormat="1" ht="24" spans="1:24">
       <c r="A56" s="17" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>37</v>
@@ -4649,18 +4654,18 @@
       <c r="W56" s="11"/>
       <c r="X56" s="11"/>
     </row>
-    <row r="57" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="57" customFormat="1" ht="36" spans="1:24">
       <c r="A57" s="17" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E57" s="11" t="s">
         <v>37</v>
@@ -4687,18 +4692,18 @@
       <c r="W57" s="11"/>
       <c r="X57" s="11"/>
     </row>
-    <row r="58" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="58" customFormat="1" ht="24" spans="1:24">
       <c r="A58" s="17" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>37</v>
@@ -4725,18 +4730,18 @@
       <c r="W58" s="11"/>
       <c r="X58" s="11"/>
     </row>
-    <row r="59" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="59" customFormat="1" ht="24" spans="1:24">
       <c r="A59" s="17" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>37</v>
@@ -4763,18 +4768,18 @@
       <c r="W59" s="11"/>
       <c r="X59" s="11"/>
     </row>
-    <row r="60" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="60" customFormat="1" ht="12" spans="1:24">
       <c r="A60" s="17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>37</v>
@@ -4801,18 +4806,18 @@
       <c r="W60" s="11"/>
       <c r="X60" s="11"/>
     </row>
-    <row r="61" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="61" customFormat="1" ht="36" spans="1:24">
       <c r="A61" s="17" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>37</v>
@@ -4841,25 +4846,25 @@
     </row>
     <row r="62" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A62" s="18" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F62" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
@@ -4881,19 +4886,19 @@
     </row>
     <row r="63" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A63" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="F63" s="7" t="b">
         <v>0</v>
@@ -4917,18 +4922,18 @@
       <c r="W63" s="7"/>
       <c r="X63" s="7"/>
     </row>
-    <row r="64" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="64" customFormat="1" ht="36" spans="1:24">
       <c r="A64" s="17" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>37</v>
@@ -4955,18 +4960,18 @@
       <c r="W64" s="11"/>
       <c r="X64" s="11"/>
     </row>
-    <row r="65" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="65" customFormat="1" ht="36" spans="1:24">
       <c r="A65" s="17" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>37</v>
@@ -4993,25 +4998,25 @@
       <c r="W65" s="11"/>
       <c r="X65" s="11"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="66" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A66" s="18" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B66" s="13"/>
       <c r="C66" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F66" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
@@ -5031,28 +5036,28 @@
       <c r="W66" s="7"/>
       <c r="X66" s="7"/>
       <c r="Y66" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="67" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A67" s="18" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B67" s="13"/>
       <c r="C67" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F67" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
@@ -5074,16 +5079,16 @@
     </row>
     <row r="68" customFormat="1" ht="12" spans="1:25">
       <c r="A68" s="17" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>37</v>
@@ -5110,35 +5115,35 @@
       <c r="W68" s="11"/>
       <c r="X68" s="11"/>
       <c r="Y68" s="37" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="69" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A69" s="18" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B69" s="13"/>
       <c r="C69" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F69" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H69" s="22" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I69" s="7"/>
       <c r="J69" s="22" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="K69" s="7"/>
       <c r="L69" s="7"/>
@@ -5155,35 +5160,35 @@
       <c r="W69" s="7"/>
       <c r="X69" s="7"/>
       <c r="Y69" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="70" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A70" s="18" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B70" s="13"/>
       <c r="C70" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F70" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H70" s="22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I70" s="7"/>
       <c r="J70" s="22" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
@@ -5200,30 +5205,30 @@
       <c r="W70" s="7"/>
       <c r="X70" s="7"/>
     </row>
-    <row r="71" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="71" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A71" s="18" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B71" s="13"/>
       <c r="C71" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F71" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="22" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
@@ -5240,35 +5245,35 @@
       <c r="W71" s="7"/>
       <c r="X71" s="7"/>
       <c r="Y71" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="72" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A72" s="18" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B72" s="13"/>
       <c r="C72" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F72" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H72" s="22" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="I72" s="7"/>
       <c r="J72" s="20" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
@@ -5285,21 +5290,21 @@
       <c r="W72" s="7"/>
       <c r="X72" s="7"/>
       <c r="Y72" s="38" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="73" customFormat="1" ht="12" hidden="1" spans="1:24">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" customFormat="1" ht="12" spans="1:24">
       <c r="A73" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B73" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>37</v>
@@ -5326,25 +5331,25 @@
       <c r="W73" s="11"/>
       <c r="X73" s="11"/>
     </row>
-    <row r="74" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="74" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A74" s="18" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B74" s="13"/>
       <c r="C74" s="7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F74" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
@@ -5364,33 +5369,33 @@
       <c r="W74" s="7"/>
       <c r="X74" s="7"/>
       <c r="Y74" s="39" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="75" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A75" s="18" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B75" s="19"/>
       <c r="C75" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F75" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="22" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
@@ -5407,19 +5412,19 @@
       <c r="W75" s="7"/>
       <c r="X75" s="7"/>
     </row>
-    <row r="76" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="76" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A76" s="7" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B76" s="16"/>
       <c r="C76" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F76" s="7" t="b">
         <v>0</v>
@@ -5443,30 +5448,30 @@
       <c r="W76" s="7"/>
       <c r="X76" s="7"/>
     </row>
-    <row r="77" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="77" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A77" s="7" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F77" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
@@ -5483,30 +5488,30 @@
       <c r="W77" s="7"/>
       <c r="X77" s="7"/>
     </row>
-    <row r="78" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="78" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A78" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F78" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
@@ -5523,30 +5528,30 @@
       <c r="W78" s="7"/>
       <c r="X78" s="7"/>
     </row>
-    <row r="79" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="79" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A79" s="7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F79" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
@@ -5563,30 +5568,30 @@
       <c r="W79" s="7"/>
       <c r="X79" s="7"/>
     </row>
-    <row r="80" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="80" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A80" s="7" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F80" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
@@ -5603,19 +5608,19 @@
       <c r="W80" s="7"/>
       <c r="X80" s="7"/>
     </row>
-    <row r="81" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="81" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A81" s="18" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B81" s="19"/>
       <c r="C81" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F81" s="7" t="b">
         <v>0</v>
@@ -5639,18 +5644,18 @@
       <c r="W81" s="7"/>
       <c r="X81" s="7"/>
     </row>
-    <row r="82" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="82" customFormat="1" ht="36" spans="1:24">
       <c r="A82" s="9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B82" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>37</v>
@@ -5677,18 +5682,18 @@
       <c r="W82" s="11"/>
       <c r="X82" s="11"/>
     </row>
-    <row r="83" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="83" customFormat="1" ht="48" spans="1:24">
       <c r="A83" s="9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B83" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E83" s="11" t="s">
         <v>37</v>
@@ -5715,18 +5720,18 @@
       <c r="W83" s="11"/>
       <c r="X83" s="11"/>
     </row>
-    <row r="84" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="84" customFormat="1" ht="36" spans="1:24">
       <c r="A84" s="9" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B84" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>37</v>
@@ -5753,18 +5758,18 @@
       <c r="W84" s="11"/>
       <c r="X84" s="11"/>
     </row>
-    <row r="85" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="85" customFormat="1" ht="24" spans="1:24">
       <c r="A85" s="9" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B85" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>37</v>
@@ -5791,18 +5796,18 @@
       <c r="W85" s="11"/>
       <c r="X85" s="11"/>
     </row>
-    <row r="86" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="86" customFormat="1" ht="24" spans="1:24">
       <c r="A86" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B86" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>37</v>
@@ -5829,18 +5834,18 @@
       <c r="W86" s="11"/>
       <c r="X86" s="11"/>
     </row>
-    <row r="87" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="87" customFormat="1" ht="24" spans="1:24">
       <c r="A87" s="9" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B87" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>37</v>
@@ -5867,21 +5872,21 @@
       <c r="W87" s="11"/>
       <c r="X87" s="11"/>
     </row>
-    <row r="88" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="88" customFormat="1" ht="24" spans="1:24">
       <c r="A88" s="7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B88" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F88" s="11" t="b">
         <v>0</v>
@@ -5905,21 +5910,21 @@
       <c r="W88" s="11"/>
       <c r="X88" s="11"/>
     </row>
-    <row r="89" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="89" customFormat="1" ht="24" spans="1:24">
       <c r="A89" s="7" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B89" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F89" s="11" t="b">
         <v>0</v>
@@ -5943,16 +5948,16 @@
       <c r="W89" s="11"/>
       <c r="X89" s="11"/>
     </row>
-    <row r="90" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="90" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A90" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>114</v>
@@ -5961,7 +5966,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
@@ -5981,18 +5986,18 @@
       <c r="W90" s="7"/>
       <c r="X90" s="7"/>
     </row>
-    <row r="91" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="91" customFormat="1" ht="36" spans="1:24">
       <c r="A91" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>37</v>
@@ -6019,16 +6024,16 @@
       <c r="W91" s="11"/>
       <c r="X91" s="11"/>
     </row>
-    <row r="92" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="92" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A92" s="7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>114</v>
@@ -6037,12 +6042,12 @@
         <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="20" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="K92" s="7"/>
       <c r="L92" s="7"/>
@@ -6059,25 +6064,25 @@
       <c r="W92" s="7"/>
       <c r="X92" s="7"/>
     </row>
-    <row r="93" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="93" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A93" s="7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F93" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G93" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
@@ -6097,25 +6102,25 @@
       <c r="W93" s="7"/>
       <c r="X93" s="7"/>
     </row>
-    <row r="94" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="94" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A94" s="7" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F94" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G94" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
@@ -6135,25 +6140,25 @@
       <c r="W94" s="7"/>
       <c r="X94" s="7"/>
     </row>
-    <row r="95" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="95" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A95" s="7" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F95" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G95" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
@@ -6173,18 +6178,18 @@
       <c r="W95" s="7"/>
       <c r="X95" s="7"/>
     </row>
-    <row r="96" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="96" customFormat="1" ht="24" spans="1:24">
       <c r="A96" s="9" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>37</v>
@@ -6211,18 +6216,18 @@
       <c r="W96" s="11"/>
       <c r="X96" s="11"/>
     </row>
-    <row r="97" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="97" customFormat="1" ht="24" spans="1:24">
       <c r="A97" s="9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>37</v>
@@ -6249,18 +6254,18 @@
       <c r="W97" s="11"/>
       <c r="X97" s="11"/>
     </row>
-    <row r="98" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="98" customFormat="1" ht="24" spans="1:24">
       <c r="A98" s="9" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>37</v>
@@ -6287,21 +6292,21 @@
       <c r="W98" s="11"/>
       <c r="X98" s="11"/>
     </row>
-    <row r="99" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="99" customFormat="1" ht="48" spans="1:24">
       <c r="A99" s="7" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B99" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F99" s="11" t="b">
         <v>0</v>
@@ -6325,28 +6330,28 @@
       <c r="W99" s="11"/>
       <c r="X99" s="11"/>
     </row>
-    <row r="100" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="100" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A100" s="7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B100" s="13"/>
       <c r="C100" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F100" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G100" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
@@ -6375,33 +6380,33 @@
       <c r="W100" s="7"/>
       <c r="X100" s="7"/>
       <c r="Y100" s="33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="101" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="101" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A101" s="7" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B101" s="13"/>
       <c r="C101" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F101" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G101" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="22" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="K101" s="7"/>
       <c r="L101" s="7"/>
@@ -6418,33 +6423,33 @@
       <c r="W101" s="7"/>
       <c r="X101" s="7"/>
       <c r="Y101" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="102" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="102" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A102" s="7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F102" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G102" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="20" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="K102" s="7"/>
       <c r="L102" s="7"/>
@@ -6461,25 +6466,25 @@
       <c r="W102" s="7"/>
       <c r="X102" s="7"/>
     </row>
-    <row r="103" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="103" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A103" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F103" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G103" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
@@ -6499,30 +6504,30 @@
       <c r="W103" s="7"/>
       <c r="X103" s="7"/>
     </row>
-    <row r="104" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="104" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A104" s="7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F104" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G104" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="20" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="K104" s="7"/>
       <c r="L104" s="7"/>
@@ -6541,19 +6546,19 @@
     </row>
     <row r="105" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A105" s="7" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F105" s="7" t="b">
         <v>0</v>
@@ -6579,25 +6584,25 @@
     </row>
     <row r="106" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A106" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B106" s="34" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F106" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G106" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
@@ -6609,7 +6614,7 @@
       <c r="O106" s="7"/>
       <c r="P106" s="7"/>
       <c r="Q106" s="7" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="R106" s="7"/>
       <c r="S106" s="7"/>
@@ -6619,9 +6624,9 @@
       <c r="W106" s="7"/>
       <c r="X106" s="7"/>
     </row>
-    <row r="107" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="107" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A107" s="7" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B107" s="16"/>
       <c r="C107" s="7"/>
@@ -6649,28 +6654,28 @@
       <c r="W107" s="7"/>
       <c r="X107" s="7"/>
     </row>
-    <row r="108" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="108" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A108" s="7" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="F108" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G108" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
@@ -6689,16 +6694,16 @@
       <c r="W108" s="7"/>
       <c r="X108" s="7"/>
     </row>
-    <row r="109" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="109" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A109" s="7" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B109" s="13"/>
       <c r="C109" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>31</v>
@@ -6707,14 +6712,14 @@
         <v>1</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H109" s="27" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="I109" s="7"/>
       <c r="J109" s="22" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="K109" s="7"/>
       <c r="L109" s="7"/>
@@ -6731,21 +6736,21 @@
       <c r="W109" s="7"/>
       <c r="X109" s="7"/>
       <c r="Y109" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="110" customFormat="1" ht="48" hidden="1" spans="1:24">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="110" customFormat="1" ht="48" spans="1:24">
       <c r="A110" s="9" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B110" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>37</v>
@@ -6772,18 +6777,18 @@
       <c r="W110" s="11"/>
       <c r="X110" s="11"/>
     </row>
-    <row r="111" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="111" customFormat="1" ht="48" spans="1:24">
       <c r="A111" s="9" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E111" s="11" t="s">
         <v>37</v>
@@ -6810,18 +6815,18 @@
       <c r="W111" s="11"/>
       <c r="X111" s="11"/>
     </row>
-    <row r="112" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="112" customFormat="1" ht="36" spans="1:24">
       <c r="A112" s="9" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E112" s="11" t="s">
         <v>37</v>
@@ -6850,18 +6855,18 @@
       <c r="W112" s="11"/>
       <c r="X112" s="11"/>
     </row>
-    <row r="113" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="113" customFormat="1" ht="36" spans="1:24">
       <c r="A113" s="9" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B113" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E113" s="11" t="s">
         <v>37</v>
@@ -6888,16 +6893,16 @@
       <c r="W113" s="11"/>
       <c r="X113" s="11"/>
     </row>
-    <row r="114" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="114" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A114" s="7" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B114" s="16"/>
       <c r="C114" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D114" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E114" s="7"/>
       <c r="F114" s="7" t="b">
@@ -6922,18 +6927,18 @@
       <c r="W114" s="7"/>
       <c r="X114" s="7"/>
     </row>
-    <row r="115" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="115" customFormat="1" ht="36" spans="1:24">
       <c r="A115" s="9" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B115" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E115" s="11" t="s">
         <v>37</v>
@@ -6960,18 +6965,18 @@
       <c r="W115" s="11"/>
       <c r="X115" s="11"/>
     </row>
-    <row r="116" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="116" customFormat="1" ht="48" spans="1:24">
       <c r="A116" s="9" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B116" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E116" s="11" t="s">
         <v>37</v>
@@ -6998,18 +7003,18 @@
       <c r="W116" s="11"/>
       <c r="X116" s="11"/>
     </row>
-    <row r="117" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="117" customFormat="1" ht="48" spans="1:24">
       <c r="A117" s="9" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B117" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>37</v>
@@ -7036,18 +7041,18 @@
       <c r="W117" s="11"/>
       <c r="X117" s="11"/>
     </row>
-    <row r="118" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="118" customFormat="1" ht="48" spans="1:24">
       <c r="A118" s="9" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B118" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>37</v>
@@ -7074,30 +7079,30 @@
       <c r="W118" s="11"/>
       <c r="X118" s="11"/>
     </row>
-    <row r="119" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="119" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A119" s="7" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B119" s="13"/>
       <c r="C119" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="F119" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G119" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="22" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="K119" s="7"/>
       <c r="L119" s="7"/>
@@ -7114,21 +7119,21 @@
       <c r="W119" s="7"/>
       <c r="X119" s="7"/>
       <c r="Y119" s="40" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="120" customFormat="1" ht="24" hidden="1" spans="1:24">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="120" customFormat="1" ht="24" spans="1:24">
       <c r="A120" s="9" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B120" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>37</v>
@@ -7155,18 +7160,18 @@
       <c r="W120" s="11"/>
       <c r="X120" s="11"/>
     </row>
-    <row r="121" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="121" customFormat="1" ht="12" spans="1:24">
       <c r="A121" s="9" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B121" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>37</v>
@@ -7193,18 +7198,18 @@
       <c r="W121" s="11"/>
       <c r="X121" s="11"/>
     </row>
-    <row r="122" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="122" customFormat="1" ht="12" spans="1:24">
       <c r="A122" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B122" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E122" s="11" t="s">
         <v>37</v>
@@ -7231,18 +7236,18 @@
       <c r="W122" s="11"/>
       <c r="X122" s="11"/>
     </row>
-    <row r="123" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="123" customFormat="1" ht="12" spans="1:24">
       <c r="A123" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B123" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E123" s="11" t="s">
         <v>37</v>
@@ -7269,18 +7274,18 @@
       <c r="W123" s="11"/>
       <c r="X123" s="11"/>
     </row>
-    <row r="124" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="124" customFormat="1" ht="12" spans="1:24">
       <c r="A124" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B124" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E124" s="11" t="s">
         <v>37</v>
@@ -7307,18 +7312,18 @@
       <c r="W124" s="11"/>
       <c r="X124" s="11"/>
     </row>
-    <row r="125" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="125" customFormat="1" ht="12" spans="1:24">
       <c r="A125" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B125" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>37</v>
@@ -7345,18 +7350,18 @@
       <c r="W125" s="11"/>
       <c r="X125" s="11"/>
     </row>
-    <row r="126" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="126" customFormat="1" ht="24" spans="1:24">
       <c r="A126" s="9" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B126" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E126" s="11" t="s">
         <v>37</v>
@@ -7383,18 +7388,18 @@
       <c r="W126" s="11"/>
       <c r="X126" s="11"/>
     </row>
-    <row r="127" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="127" customFormat="1" ht="12" spans="1:24">
       <c r="A127" s="9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B127" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E127" s="11" t="s">
         <v>37</v>
@@ -7421,28 +7426,28 @@
       <c r="W127" s="11"/>
       <c r="X127" s="11"/>
     </row>
-    <row r="128" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="128" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A128" s="7" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="F128" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G128" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="H128" s="35" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
@@ -7461,25 +7466,25 @@
       <c r="W128" s="7"/>
       <c r="X128" s="7"/>
     </row>
-    <row r="129" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="129" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A129" s="7" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F129" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G129" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
@@ -7499,18 +7504,18 @@
       <c r="W129" s="7"/>
       <c r="X129" s="7"/>
     </row>
-    <row r="130" customFormat="1" ht="36" hidden="1" spans="1:24">
+    <row r="130" customFormat="1" ht="36" spans="1:24">
       <c r="A130" s="9" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B130" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C130" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>37</v>
@@ -7537,18 +7542,18 @@
       <c r="W130" s="11"/>
       <c r="X130" s="11"/>
     </row>
-    <row r="131" customFormat="1" ht="48" hidden="1" spans="1:24">
+    <row r="131" customFormat="1" ht="48" spans="1:24">
       <c r="A131" s="9" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B131" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E131" s="11" t="s">
         <v>37</v>
@@ -7575,25 +7580,25 @@
       <c r="W131" s="11"/>
       <c r="X131" s="11"/>
     </row>
-    <row r="132" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+    <row r="132" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A132" s="7" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B132" s="13"/>
       <c r="C132" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D132" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F132" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G132" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
@@ -7613,28 +7618,28 @@
       <c r="W132" s="7"/>
       <c r="X132" s="7"/>
       <c r="Y132" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="133" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="133" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A133" s="7" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F133" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G133" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
@@ -7654,28 +7659,28 @@
       <c r="W133" s="7"/>
       <c r="X133" s="7"/>
       <c r="Y133" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="134" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="134" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A134" s="7" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B134" s="13"/>
       <c r="C134" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F134" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G134" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
@@ -7695,21 +7700,21 @@
       <c r="W134" s="7"/>
       <c r="X134" s="7"/>
       <c r="Y134" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A135" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E135" s="7" t="s">
         <v>48</v>
@@ -7718,12 +7723,12 @@
         <v>0</v>
       </c>
       <c r="G135" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" s="22" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="K135" s="7"/>
       <c r="L135" s="7"/>
@@ -7741,22 +7746,22 @@
       <c r="V135" s="7"/>
       <c r="W135" s="7"/>
       <c r="X135" s="7"/>
-      <c r="Y135" s="43" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="136" customFormat="1" ht="24" hidden="1" spans="1:24">
+      <c r="Y135" s="42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="136" customFormat="1" ht="24" spans="1:24">
       <c r="A136" s="17" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B136" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>37</v>
@@ -7783,16 +7788,16 @@
       <c r="W136" s="11"/>
       <c r="X136" s="11"/>
     </row>
-    <row r="137" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="137" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A137" s="18" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B137" s="13"/>
       <c r="C137" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>114</v>
@@ -7821,16 +7826,16 @@
       <c r="W137" s="7"/>
       <c r="X137" s="7"/>
     </row>
-    <row r="138" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="138" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A138" s="7" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B138" s="16"/>
       <c r="C138" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E138" s="7" t="s">
         <v>48</v>
@@ -7856,19 +7861,19 @@
       <c r="V138" s="7"/>
       <c r="W138" s="7"/>
       <c r="X138" s="7" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="139" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="139" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A139" s="7" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B139" s="16"/>
       <c r="C139" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E139" s="7" t="s">
         <v>31</v>
@@ -7880,7 +7885,7 @@
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" s="20" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="K139" s="7"/>
       <c r="L139" s="7"/>
@@ -7897,19 +7902,19 @@
       <c r="W139" s="7"/>
       <c r="X139" s="7"/>
     </row>
-    <row r="140" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="140" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A140" s="7" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B140" s="16"/>
       <c r="C140" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E140" s="7" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="F140" s="7" t="b">
         <v>1</v>
@@ -7934,28 +7939,28 @@
       <c r="V140" s="7"/>
       <c r="W140" s="7"/>
       <c r="X140" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="141" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="141" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A141" s="7" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B141" s="8"/>
       <c r="C141" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F141" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G141" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
@@ -7974,33 +7979,33 @@
       <c r="V141" s="7"/>
       <c r="W141" s="7"/>
       <c r="X141" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="142" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="142" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A142" s="7" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B142" s="8"/>
       <c r="C142" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E142" s="7" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F142" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G142" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" s="22" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="K142" s="7"/>
       <c r="L142" s="7"/>
@@ -8016,28 +8021,28 @@
       <c r="V142" s="7"/>
       <c r="W142" s="7"/>
       <c r="X142" s="7" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="143" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="143" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A143" s="7" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F143" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G143" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
@@ -8056,21 +8061,21 @@
       <c r="V143" s="7"/>
       <c r="W143" s="7"/>
       <c r="X143" s="7" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="144" customFormat="1" ht="24" hidden="1" spans="1:24">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="144" customFormat="1" ht="24" spans="1:24">
       <c r="A144" s="9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B144" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E144" s="11" t="s">
         <v>37</v>
@@ -8097,25 +8102,25 @@
       <c r="W144" s="11"/>
       <c r="X144" s="11"/>
     </row>
-    <row r="145" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="145" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A145" s="7" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B145" s="8"/>
       <c r="C145" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F145" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G145" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -8135,18 +8140,18 @@
       <c r="W145" s="7"/>
       <c r="X145" s="7"/>
     </row>
-    <row r="146" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="146" customFormat="1" ht="24" spans="1:24">
       <c r="A146" s="9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B146" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D146" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E146" s="11" t="s">
         <v>37</v>
@@ -8172,19 +8177,19 @@
       <c r="V146" s="11"/>
       <c r="W146" s="11"/>
       <c r="X146" s="11" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="147" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="147" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A147" s="7" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B147" s="8"/>
       <c r="C147" s="7" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>52</v>
@@ -8193,7 +8198,7 @@
         <v>1</v>
       </c>
       <c r="G147" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
@@ -8214,28 +8219,28 @@
       <c r="V147" s="7"/>
       <c r="W147" s="7"/>
       <c r="X147" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="148" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="148" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A148" s="7" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B148" s="8"/>
       <c r="C148" s="7" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D148" s="7" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E148" s="7" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="F148" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G148" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="H148" s="7"/>
       <c r="I148" s="7"/>
@@ -8257,23 +8262,23 @@
     </row>
     <row r="149" s="1" customFormat="1" ht="100" customHeight="1" spans="1:25">
       <c r="A149" s="7" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B149" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E149" s="7"/>
       <c r="F149" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G149" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
@@ -8292,31 +8297,31 @@
       <c r="V149" s="7"/>
       <c r="W149" s="7"/>
       <c r="X149" s="7"/>
-      <c r="Y149" s="43" t="s">
-        <v>387</v>
+      <c r="Y149" s="42" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A150" s="7" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B150" s="41" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F150" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G150" s="42" t="s">
-        <v>365</v>
+      <c r="G150" s="25" t="s">
+        <v>367</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
@@ -8338,23 +8343,23 @@
     </row>
     <row r="151" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A151" s="7" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B151" s="41"/>
       <c r="C151" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F151" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G151" s="42" t="s">
-        <v>365</v>
+      <c r="G151" s="25" t="s">
+        <v>367</v>
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
@@ -8376,17 +8381,17 @@
     </row>
     <row r="152" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A152" s="7" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B152" s="41"/>
       <c r="C152" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D152" s="7" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E152" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F152" s="7" t="b">
         <v>0</v>
@@ -8412,17 +8417,17 @@
     </row>
     <row r="153" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A153" s="7" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B153" s="41"/>
       <c r="C153" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D153" s="7" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F153" s="7" t="b">
         <v>0</v>
@@ -8448,28 +8453,28 @@
     </row>
     <row r="154" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A154" s="7" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B154" s="16"/>
       <c r="C154" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D154" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E154" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F154" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="7"/>
       <c r="J154" s="20" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="K154" s="7"/>
       <c r="L154" s="7"/>
@@ -8488,23 +8493,23 @@
     </row>
     <row r="155" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A155" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B155" s="16"/>
       <c r="C155" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F155" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G155" s="5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
@@ -8526,17 +8531,17 @@
     </row>
     <row r="156" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A156" s="7" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B156" s="41"/>
       <c r="C156" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D156" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F156" s="7" t="b">
         <v>0</v>
@@ -8562,14 +8567,14 @@
     </row>
     <row r="157" customFormat="1" ht="24" spans="1:24">
       <c r="A157" s="9" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B157" s="16"/>
       <c r="C157" s="11" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E157" s="11" t="s">
         <v>37</v>
@@ -8598,17 +8603,17 @@
     </row>
     <row r="158" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A158" s="7" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B158" s="41"/>
       <c r="C158" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D158" s="7" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F158" s="7" t="b">
         <v>0</v>
@@ -8632,18 +8637,18 @@
       <c r="W158" s="7"/>
       <c r="X158" s="7"/>
     </row>
-    <row r="159" customFormat="1" ht="12" hidden="1" spans="1:24">
+    <row r="159" customFormat="1" ht="12" spans="1:24">
       <c r="A159" s="9" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B159" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>37</v>
@@ -8670,30 +8675,30 @@
       <c r="W159" s="11"/>
       <c r="X159" s="11"/>
     </row>
-    <row r="160" s="1" customFormat="1" ht="100" hidden="1" customHeight="1" spans="1:24">
+    <row r="160" s="1" customFormat="1" ht="100" customHeight="1" spans="1:24">
       <c r="A160" s="7" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B160" s="8"/>
       <c r="C160" s="7" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F160" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G160" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
       <c r="J160" s="20" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K160" s="7"/>
       <c r="L160" s="7"/>
@@ -8707,23 +8712,23 @@
       <c r="T160" s="7"/>
       <c r="U160" s="7"/>
       <c r="V160" s="7" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="W160" s="7"/>
       <c r="X160" s="7"/>
     </row>
-    <row r="161" customFormat="1" ht="24" hidden="1" spans="1:24">
+    <row r="161" customFormat="1" ht="24" spans="1:24">
       <c r="A161" s="9" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B161" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>37</v>
@@ -33997,22 +34002,7 @@
       <c r="X1132" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y161">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="cant find data"/>
-        <filter val="platform no csv/xlsx found pdf report of processed data"/>
-        <filter val="data interactive and dynamic"/>
-        <filter val="wrong format"/>
-        <filter val="WIDGET"/>
-        <filter val="not sure where data is located"/>
-        <filter val="zip file not working"/>
-        <filter val="txt not working"/>
-        <filter val="requires login info"/>
-        <filter val="needs registration and to book a demo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Y161"/>
   <mergeCells count="1">
     <mergeCell ref="B150:B158"/>
   </mergeCells>

</xml_diff>

<commit_message>
Further additions for the framework
</commit_message>
<xml_diff>
--- a/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
+++ b/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stan Smith\Documents\GIT\UNDP\digital-readiness-assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A35FBBE-8235-405A-B81D-03247C9F2DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3116F00-0DD1-48F3-8B67-131236770DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="495">
   <si>
     <t>Indicator</t>
   </si>
@@ -1277,9 +1277,6 @@
   </si>
   <si>
     <t>Speedtest Global Index</t>
-  </si>
-  <si>
-    <t>UN</t>
   </si>
   <si>
     <t>population_density</t>
@@ -1536,12 +1533,56 @@
 Source: World Bank, Global Findex database    (https://globalfindex.worldbank.org/)
 For some countries, the latest year for which data are available may differ from the year that appears at the top of the page. The cut-off year is 2009.</t>
   </si>
+  <si>
+    <t>36 countries only</t>
+  </si>
+  <si>
+    <t>Boston Consulting Group/SalesForce</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Q. Which of the following best </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>describes how well current online government services meet your need?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1. Needs Never Met, 2. Needs often not met,
+3. Needs sometimes met, 4. Most needs met, 5. All Needs Met. 
+Net Perception = total needs most or always met (4 and 5) – needs often not met or never
+met (1 and 2). In calculating net perception 3 was neutral.
+Source : BCG 2020 Digital Government Citizen Survey</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.salesforce.com/wbin/sfdc-www/autodownloadpdf?path=%2F%2Fwww.salesforce.com%2Fcontent%2Fdam%2Fweb%2Fen_sg%2Fwww%2Fdocuments%2Fpdf%2Fthe-global-trust-imperative.pdf</t>
+  </si>
+  <si>
+    <t>Only 36 countries</t>
+  </si>
+  <si>
+    <t>digital_public_service_use</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1675,6 +1716,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1838,16 +1886,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2071,11 +2119,11 @@
   </sheetPr>
   <dimension ref="A1:Y1134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C127" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H132" sqref="H132"/>
+      <selection pane="bottomRight" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2296,10 +2344,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="H5" s="39" t="s">
         <v>414</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>415</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -2338,10 +2386,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H6" s="39" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -2801,7 +2849,7 @@
       <c r="A18" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="11" t="s">
         <v>35</v>
       </c>
@@ -2809,16 +2857,16 @@
         <v>36</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F18" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G18" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="H18" s="39" t="s">
         <v>419</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>420</v>
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -2889,18 +2937,18 @@
         <v>36</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F20" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="11"/>
       <c r="J20" s="39" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -3418,7 +3466,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>35</v>
@@ -3430,15 +3478,15 @@
         <v>52</v>
       </c>
       <c r="F33" s="44" t="s">
+        <v>469</v>
+      </c>
+      <c r="G33" s="41" t="s">
         <v>470</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>471</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -3829,20 +3877,20 @@
         <v>141</v>
       </c>
       <c r="E43" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="H43" s="46" t="s">
         <v>485</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="H43" s="48" t="s">
-        <v>486</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="39" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
@@ -4403,12 +4451,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:25" customFormat="1" ht="52.8">
+    <row r="57" spans="1:25" customFormat="1" ht="179.4" customHeight="1">
       <c r="A57" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>34</v>
+      <c r="B57" s="6" t="s">
+        <v>489</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>167</v>
@@ -4417,15 +4465,21 @@
         <v>168</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>413</v>
+        <v>490</v>
       </c>
       <c r="F57" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
+      <c r="G57" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>491</v>
+      </c>
       <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
+      <c r="J57" s="39" t="s">
+        <v>492</v>
+      </c>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
@@ -4441,7 +4495,7 @@
       <c r="W57" s="11"/>
       <c r="X57" s="11"/>
     </row>
-    <row r="58" spans="1:25" customFormat="1" ht="26.4">
+    <row r="58" spans="1:25" customFormat="1" ht="39.6">
       <c r="A58" s="16" t="s">
         <v>180</v>
       </c>
@@ -4479,7 +4533,7 @@
       <c r="W58" s="11"/>
       <c r="X58" s="11"/>
     </row>
-    <row r="59" spans="1:25" customFormat="1" ht="39.6">
+    <row r="59" spans="1:25" customFormat="1" ht="66">
       <c r="A59" s="16" t="s">
         <v>181</v>
       </c>
@@ -4537,10 +4591,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H60" s="39" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
@@ -4559,7 +4613,7 @@
       <c r="W60" s="11"/>
       <c r="X60" s="11"/>
     </row>
-    <row r="61" spans="1:25" customFormat="1" ht="118.8">
+    <row r="61" spans="1:25" customFormat="1" ht="145.19999999999999">
       <c r="A61" s="16" t="s">
         <v>184</v>
       </c>
@@ -4573,16 +4627,16 @@
         <v>183</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F61" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G61" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="H61" s="39" t="s">
         <v>424</v>
-      </c>
-      <c r="H61" s="39" t="s">
-        <v>425</v>
       </c>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
@@ -4601,7 +4655,7 @@
       <c r="W61" s="11"/>
       <c r="X61" s="11"/>
     </row>
-    <row r="62" spans="1:25" customFormat="1" ht="13.2">
+    <row r="62" spans="1:25" customFormat="1" ht="26.4">
       <c r="A62" s="16" t="s">
         <v>185</v>
       </c>
@@ -4755,7 +4809,7 @@
       <c r="W65" s="7"/>
       <c r="X65" s="7"/>
     </row>
-    <row r="66" spans="1:25" customFormat="1" ht="39.6">
+    <row r="66" spans="1:25" customFormat="1" ht="52.8">
       <c r="A66" s="16" t="s">
         <v>194</v>
       </c>
@@ -4793,7 +4847,7 @@
       <c r="W66" s="11"/>
       <c r="X66" s="11"/>
     </row>
-    <row r="67" spans="1:25" customFormat="1" ht="66">
+    <row r="67" spans="1:25" customFormat="1" ht="79.2">
       <c r="A67" s="16" t="s">
         <v>195</v>
       </c>
@@ -4807,20 +4861,20 @@
         <v>196</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F67" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I67" s="11"/>
       <c r="J67" s="39" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
@@ -5485,7 +5539,7 @@
       <c r="W83" s="7"/>
       <c r="X83" s="7"/>
     </row>
-    <row r="84" spans="1:24" customFormat="1" ht="39.6">
+    <row r="84" spans="1:24" customFormat="1" ht="52.8">
       <c r="A84" s="9" t="s">
         <v>252</v>
       </c>
@@ -5523,7 +5577,7 @@
       <c r="W84" s="11"/>
       <c r="X84" s="11"/>
     </row>
-    <row r="85" spans="1:24" customFormat="1" ht="52.8">
+    <row r="85" spans="1:24" customFormat="1" ht="66">
       <c r="A85" s="9" t="s">
         <v>253</v>
       </c>
@@ -5637,12 +5691,12 @@
       <c r="W87" s="11"/>
       <c r="X87" s="11"/>
     </row>
-    <row r="88" spans="1:24" customFormat="1" ht="52.8">
+    <row r="88" spans="1:24" customFormat="1" ht="66">
       <c r="A88" s="9" t="s">
         <v>256</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C88" s="11" t="s">
         <v>238</v>
@@ -5657,12 +5711,12 @@
         <v>0</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="11"/>
       <c r="J88" s="39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K88" s="11"/>
       <c r="L88" s="11"/>
@@ -5691,20 +5745,20 @@
         <v>239</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F89" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="39" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K89" s="11"/>
       <c r="L89" s="11"/>
@@ -5721,7 +5775,7 @@
       <c r="W89" s="11"/>
       <c r="X89" s="11"/>
     </row>
-    <row r="90" spans="1:24" customFormat="1" ht="52.8">
+    <row r="90" spans="1:24" customFormat="1" ht="66">
       <c r="A90" s="7" t="s">
         <v>258</v>
       </c>
@@ -5733,20 +5787,20 @@
         <v>239</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F90" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G90" s="41" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I90" s="11"/>
       <c r="J90" s="39" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K90" s="11"/>
       <c r="L90" s="11"/>
@@ -5763,7 +5817,7 @@
       <c r="W90" s="11"/>
       <c r="X90" s="11"/>
     </row>
-    <row r="91" spans="1:24" customFormat="1" ht="52.8">
+    <row r="91" spans="1:24" customFormat="1" ht="66">
       <c r="A91" s="7" t="s">
         <v>259</v>
       </c>
@@ -5775,20 +5829,20 @@
         <v>239</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F91" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G91" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="H91" s="7" t="s">
         <v>478</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>479</v>
       </c>
       <c r="I91" s="11"/>
       <c r="J91" s="39" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K91" s="11"/>
       <c r="L91" s="11"/>
@@ -5843,7 +5897,7 @@
       <c r="W92" s="7"/>
       <c r="X92" s="7"/>
     </row>
-    <row r="93" spans="1:24" customFormat="1" ht="39.6">
+    <row r="93" spans="1:24" customFormat="1" ht="66">
       <c r="A93" s="9" t="s">
         <v>263</v>
       </c>
@@ -6073,7 +6127,7 @@
       <c r="W98" s="11"/>
       <c r="X98" s="11"/>
     </row>
-    <row r="99" spans="1:25" customFormat="1" ht="26.4">
+    <row r="99" spans="1:25" customFormat="1" ht="39.6">
       <c r="A99" s="9" t="s">
         <v>277</v>
       </c>
@@ -6111,7 +6165,7 @@
       <c r="W99" s="11"/>
       <c r="X99" s="11"/>
     </row>
-    <row r="100" spans="1:25" customFormat="1" ht="66">
+    <row r="100" spans="1:25" customFormat="1" ht="79.2">
       <c r="A100" s="9" t="s">
         <v>278</v>
       </c>
@@ -6131,14 +6185,14 @@
         <v>0</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I100" s="11"/>
       <c r="J100" s="39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K100" s="11"/>
       <c r="L100" s="11"/>
@@ -6155,12 +6209,12 @@
       <c r="W100" s="11"/>
       <c r="X100" s="11"/>
     </row>
-    <row r="101" spans="1:25" customFormat="1" ht="52.8">
+    <row r="101" spans="1:25" customFormat="1" ht="66">
       <c r="A101" s="7" t="s">
         <v>279</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C101" s="11" t="s">
         <v>238</v>
@@ -6169,16 +6223,16 @@
         <v>266</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F101" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G101" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="H101" s="39" t="s">
         <v>447</v>
-      </c>
-      <c r="H101" s="39" t="s">
-        <v>448</v>
       </c>
       <c r="I101" s="11"/>
       <c r="J101" s="11"/>
@@ -6416,7 +6470,7 @@
         <v>296</v>
       </c>
       <c r="B107" s="42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>281</v>
@@ -6425,18 +6479,18 @@
         <v>282</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F107" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="39" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K107" s="7"/>
       <c r="L107" s="7"/>
@@ -6471,10 +6525,10 @@
         <v>0</v>
       </c>
       <c r="G108" t="s">
+        <v>453</v>
+      </c>
+      <c r="H108" s="39" t="s">
         <v>454</v>
-      </c>
-      <c r="H108" s="39" t="s">
-        <v>455</v>
       </c>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
@@ -6648,12 +6702,12 @@
       <c r="W112" s="11"/>
       <c r="X112" s="11"/>
     </row>
-    <row r="113" spans="1:25" customFormat="1" ht="52.8">
+    <row r="113" spans="1:25" customFormat="1" ht="145.19999999999999">
       <c r="A113" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="B113" s="10" t="s">
-        <v>34</v>
+      <c r="B113" s="6" t="s">
+        <v>493</v>
       </c>
       <c r="C113" s="11" t="s">
         <v>281</v>
@@ -6662,15 +6716,21 @@
         <v>302</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>37</v>
+        <v>490</v>
       </c>
       <c r="F113" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="G113" s="7"/>
-      <c r="H113" s="7"/>
+      <c r="G113" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>491</v>
+      </c>
       <c r="I113" s="11"/>
-      <c r="J113" s="11"/>
+      <c r="J113" s="39" t="s">
+        <v>492</v>
+      </c>
       <c r="K113" s="11"/>
       <c r="L113" s="11"/>
       <c r="M113" s="11"/>
@@ -6686,7 +6746,7 @@
       <c r="W113" s="11"/>
       <c r="X113" s="11"/>
     </row>
-    <row r="114" spans="1:25" customFormat="1" ht="39.6">
+    <row r="114" spans="1:25" customFormat="1" ht="52.8">
       <c r="A114" s="9" t="s">
         <v>313</v>
       </c>
@@ -6706,12 +6766,12 @@
         <v>1</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="11"/>
       <c r="J114" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K114" s="11"/>
       <c r="L114" s="11"/>
@@ -6728,7 +6788,7 @@
       <c r="W114" s="11"/>
       <c r="X114" s="11"/>
     </row>
-    <row r="115" spans="1:25" customFormat="1" ht="52.8">
+    <row r="115" spans="1:25" customFormat="1" ht="66">
       <c r="A115" s="9" t="s">
         <v>314</v>
       </c>
@@ -6740,18 +6800,18 @@
         <v>315</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F115" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="11"/>
       <c r="J115" s="39" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K115" s="11"/>
       <c r="L115" s="11"/>
@@ -6802,7 +6862,7 @@
       <c r="W116" s="7"/>
       <c r="X116" s="7"/>
     </row>
-    <row r="117" spans="1:25" customFormat="1" ht="39.6">
+    <row r="117" spans="1:25" customFormat="1" ht="66">
       <c r="A117" s="9" t="s">
         <v>317</v>
       </c>
@@ -6840,7 +6900,7 @@
       <c r="W117" s="11"/>
       <c r="X117" s="11"/>
     </row>
-    <row r="118" spans="1:25" customFormat="1" ht="52.8">
+    <row r="118" spans="1:25" customFormat="1" ht="79.2">
       <c r="A118" s="9" t="s">
         <v>318</v>
       </c>
@@ -6916,7 +6976,7 @@
       <c r="W119" s="11"/>
       <c r="X119" s="11"/>
     </row>
-    <row r="120" spans="1:25" customFormat="1" ht="52.8">
+    <row r="120" spans="1:25" customFormat="1" ht="66">
       <c r="A120" s="9" t="s">
         <v>320</v>
       </c>
@@ -7035,7 +7095,7 @@
       <c r="W122" s="11"/>
       <c r="X122" s="11"/>
     </row>
-    <row r="123" spans="1:25" customFormat="1" ht="13.2">
+    <row r="123" spans="1:25" customFormat="1" ht="26.4">
       <c r="A123" s="9" t="s">
         <v>327</v>
       </c>
@@ -7111,7 +7171,7 @@
       <c r="W124" s="11"/>
       <c r="X124" s="11"/>
     </row>
-    <row r="125" spans="1:25" customFormat="1" ht="13.2">
+    <row r="125" spans="1:25" customFormat="1" ht="26.4">
       <c r="A125" s="9" t="s">
         <v>329</v>
       </c>
@@ -7163,18 +7223,18 @@
         <v>315</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F126" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H126" s="1"/>
       <c r="I126" s="11"/>
       <c r="J126" s="39" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K126" s="11"/>
       <c r="L126" s="11"/>
@@ -7267,7 +7327,7 @@
       <c r="W128" s="11"/>
       <c r="X128" s="11"/>
     </row>
-    <row r="129" spans="1:25" customFormat="1" ht="13.2">
+    <row r="129" spans="1:25" customFormat="1" ht="26.4">
       <c r="A129" s="9" t="s">
         <v>333</v>
       </c>
@@ -7383,7 +7443,7 @@
       <c r="W131" s="7"/>
       <c r="X131" s="7"/>
     </row>
-    <row r="132" spans="1:25" customFormat="1" ht="105.6">
+    <row r="132" spans="1:25" customFormat="1" ht="118.8">
       <c r="A132" s="9" t="s">
         <v>342</v>
       </c>
@@ -7395,20 +7455,20 @@
         <v>339</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F132" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G132" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="H132" s="7" t="s">
         <v>488</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>489</v>
       </c>
       <c r="I132" s="11"/>
       <c r="J132" s="39" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K132" s="11"/>
       <c r="L132" s="11"/>
@@ -7425,7 +7485,7 @@
       <c r="W132" s="11"/>
       <c r="X132" s="11"/>
     </row>
-    <row r="133" spans="1:25" customFormat="1" ht="66">
+    <row r="133" spans="1:25" customFormat="1" ht="92.4">
       <c r="A133" s="9" t="s">
         <v>343</v>
       </c>
@@ -7437,20 +7497,20 @@
         <v>339</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F133" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I133" s="11"/>
       <c r="J133" s="39" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K133" s="11"/>
       <c r="L133" s="11"/>
@@ -7608,12 +7668,12 @@
         <v>1</v>
       </c>
       <c r="G137" s="41" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K137" s="7"/>
       <c r="L137" s="7"/>
@@ -7655,12 +7715,12 @@
         <v>1</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="11"/>
       <c r="J138" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K138" s="11"/>
       <c r="L138" s="11"/>
@@ -7698,7 +7758,7 @@
         <v>356</v>
       </c>
       <c r="H139" s="39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -7735,12 +7795,12 @@
         <v>0</v>
       </c>
       <c r="G140" s="41" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
       <c r="J140" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K140" s="7"/>
       <c r="L140" s="7"/>
@@ -7771,18 +7831,18 @@
         <v>339</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F141" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K141" s="7"/>
       <c r="L141" s="7"/>
@@ -7817,12 +7877,12 @@
         <v>1</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K142" s="7"/>
       <c r="L142" s="7"/>
@@ -7983,10 +8043,10 @@
         <v>0</v>
       </c>
       <c r="G146" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H146" s="39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I146" s="11"/>
       <c r="J146" s="11"/>
@@ -8063,10 +8123,10 @@
         <v>0</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H148" s="39" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I148" s="11"/>
       <c r="J148" s="11"/>
@@ -8212,7 +8272,7 @@
       <c r="A152" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="B152" s="45" t="s">
+      <c r="B152" s="47" t="s">
         <v>387</v>
       </c>
       <c r="C152" s="7" t="s">
@@ -8252,7 +8312,7 @@
       <c r="A153" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="B153" s="45"/>
+      <c r="B153" s="47"/>
       <c r="C153" s="7" t="s">
         <v>382</v>
       </c>
@@ -8290,7 +8350,7 @@
       <c r="A154" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="B154" s="45"/>
+      <c r="B154" s="47"/>
       <c r="C154" s="7" t="s">
         <v>382</v>
       </c>
@@ -8326,7 +8386,7 @@
       <c r="A155" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="B155" s="45"/>
+      <c r="B155" s="47"/>
       <c r="C155" s="7" t="s">
         <v>382</v>
       </c>
@@ -8362,7 +8422,7 @@
       <c r="A156" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="B156" s="46"/>
+      <c r="B156" s="48"/>
       <c r="C156" s="7" t="s">
         <v>382</v>
       </c>
@@ -8402,7 +8462,7 @@
       <c r="A157" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="B157" s="46"/>
+      <c r="B157" s="48"/>
       <c r="C157" s="7" t="s">
         <v>382</v>
       </c>
@@ -8440,7 +8500,7 @@
       <c r="A158" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="B158" s="45"/>
+      <c r="B158" s="47"/>
       <c r="C158" s="7" t="s">
         <v>382</v>
       </c>
@@ -8478,7 +8538,7 @@
       <c r="A159" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="B159" s="46"/>
+      <c r="B159" s="48"/>
       <c r="C159" s="11" t="s">
         <v>382</v>
       </c>
@@ -8516,7 +8576,7 @@
       <c r="A160" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="B160" s="45"/>
+      <c r="B160" s="47"/>
       <c r="C160" s="7" t="s">
         <v>382</v>
       </c>
@@ -8550,7 +8610,7 @@
       <c r="W160" s="7"/>
       <c r="X160" s="7"/>
     </row>
-    <row r="161" spans="1:24" customFormat="1" ht="26.4">
+    <row r="161" spans="1:24" customFormat="1" ht="13.2">
       <c r="A161" s="9" t="s">
         <v>399</v>
       </c>
@@ -33994,20 +34054,22 @@
     <hyperlink ref="H148" r:id="rId72" xr:uid="{D940A82C-9AE8-4B26-8FBD-7AB3C80868B6}"/>
     <hyperlink ref="H146" r:id="rId73" xr:uid="{14B4713A-90DC-43C2-93CF-F91D53FEF229}"/>
     <hyperlink ref="H139" r:id="rId74" xr:uid="{DF3A9169-5280-4EEC-AC1A-C4032C9D9F11}"/>
-    <hyperlink ref="J126" r:id="rId75" xr:uid="{E0AEEA8C-5280-4725-B3FD-AD8ED2BD872C}"/>
-    <hyperlink ref="J100" r:id="rId76" location="table-link" xr:uid="{6E54A5EC-22A9-47C5-9003-55CE4B600142}"/>
-    <hyperlink ref="H101" r:id="rId77" xr:uid="{D2CA9562-70F9-4E79-86A5-25CB85F5EAF6}"/>
-    <hyperlink ref="J107" r:id="rId78" xr:uid="{FAE0DD1D-4712-4CEF-B576-E6084ACB6287}"/>
-    <hyperlink ref="H108" r:id="rId79" xr:uid="{ECB1D51B-3320-466D-990D-5C4DCBD6D0A0}"/>
-    <hyperlink ref="J115" r:id="rId80" xr:uid="{90D5133A-C422-4E5C-A969-A0130C0192D1}"/>
-    <hyperlink ref="J133" r:id="rId81" xr:uid="{288224BA-0C98-4642-B828-98C9BA5F2561}"/>
-    <hyperlink ref="J20" r:id="rId82" location="year=2019&amp;dataSet=dimension" xr:uid="{363B7758-921D-4679-898F-19B30A88B33C}"/>
-    <hyperlink ref="J89" r:id="rId83" xr:uid="{9CDA529A-A05D-4F39-8066-D63F247DD8F0}"/>
-    <hyperlink ref="J90" r:id="rId84" xr:uid="{4C26B9A3-A75B-471F-8E98-11536DA92CCB}"/>
-    <hyperlink ref="J91" r:id="rId85" xr:uid="{00EEB2F6-E536-41E3-89F0-13FFDA331D9B}"/>
-    <hyperlink ref="J88" r:id="rId86" xr:uid="{FE175305-783C-4F64-B2D2-4097F8464B10}"/>
-    <hyperlink ref="J43" r:id="rId87" xr:uid="{4038F602-BCD0-4151-A01B-3F8D616E5B7C}"/>
-    <hyperlink ref="J132" r:id="rId88" xr:uid="{993D0A10-BA59-41C6-9FF0-BF836B389003}"/>
+    <hyperlink ref="J100" r:id="rId75" location="table-link" xr:uid="{6E54A5EC-22A9-47C5-9003-55CE4B600142}"/>
+    <hyperlink ref="H101" r:id="rId76" xr:uid="{D2CA9562-70F9-4E79-86A5-25CB85F5EAF6}"/>
+    <hyperlink ref="J107" r:id="rId77" xr:uid="{FAE0DD1D-4712-4CEF-B576-E6084ACB6287}"/>
+    <hyperlink ref="H108" r:id="rId78" xr:uid="{ECB1D51B-3320-466D-990D-5C4DCBD6D0A0}"/>
+    <hyperlink ref="J115" r:id="rId79" xr:uid="{90D5133A-C422-4E5C-A969-A0130C0192D1}"/>
+    <hyperlink ref="J133" r:id="rId80" xr:uid="{288224BA-0C98-4642-B828-98C9BA5F2561}"/>
+    <hyperlink ref="J20" r:id="rId81" location="year=2019&amp;dataSet=dimension" xr:uid="{363B7758-921D-4679-898F-19B30A88B33C}"/>
+    <hyperlink ref="J89" r:id="rId82" xr:uid="{9CDA529A-A05D-4F39-8066-D63F247DD8F0}"/>
+    <hyperlink ref="J90" r:id="rId83" xr:uid="{4C26B9A3-A75B-471F-8E98-11536DA92CCB}"/>
+    <hyperlink ref="J91" r:id="rId84" xr:uid="{00EEB2F6-E536-41E3-89F0-13FFDA331D9B}"/>
+    <hyperlink ref="J88" r:id="rId85" xr:uid="{FE175305-783C-4F64-B2D2-4097F8464B10}"/>
+    <hyperlink ref="J43" r:id="rId86" xr:uid="{4038F602-BCD0-4151-A01B-3F8D616E5B7C}"/>
+    <hyperlink ref="J132" r:id="rId87" xr:uid="{993D0A10-BA59-41C6-9FF0-BF836B389003}"/>
+    <hyperlink ref="J57" r:id="rId88" xr:uid="{2EE07639-D1D0-49A0-A8E7-464240B67E40}"/>
+    <hyperlink ref="J126" r:id="rId89" xr:uid="{E0AEEA8C-5280-4725-B3FD-AD8ED2BD872C}"/>
+    <hyperlink ref="J113" r:id="rId90" xr:uid="{73C7F521-6919-4811-A9E4-7190D7911351}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="120" orientation="portrait"/>

</xml_diff>

<commit_message>
Update UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
</commit_message>
<xml_diff>
--- a/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
+++ b/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stan Smith\Documents\GIT\UNDP\digital-readiness-assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAFD9F4-47DC-48A2-8EF5-7313D67A8650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A32C45-93F5-43FC-9697-AAB64CC06556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="512">
   <si>
     <t>Indicator</t>
   </si>
@@ -762,9 +762,6 @@
   </si>
   <si>
     <t>Networking Services (Spend, IT Forecast Data)</t>
-  </si>
-  <si>
-    <t>Gartner</t>
   </si>
   <si>
     <t xml:space="preserve">ICT goods exports </t>
@@ -1627,6 +1624,12 @@
   </si>
   <si>
     <t>https://api.worldbank.org/v2/en/indicator/IT.NET.USER.ZS?downloadformat=excel</t>
+  </si>
+  <si>
+    <t>network_readiness_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Network Readiness Index combines network quality metrics (cost, speed, coverage) with government policies as well as the impact of these factors on society as a whole. </t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1948,6 +1951,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2176,11 +2182,11 @@
   </sheetPr>
   <dimension ref="A1:Y1134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2401,10 +2407,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H5" s="39" t="s">
         <v>412</v>
-      </c>
-      <c r="H5" s="39" t="s">
-        <v>413</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -2443,10 +2449,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H6" s="39" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -2563,10 +2569,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="H9" s="39" t="s">
         <v>509</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>510</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
@@ -2916,16 +2922,16 @@
         <v>36</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F18" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G18" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="H18" s="39" t="s">
         <v>417</v>
-      </c>
-      <c r="H18" s="39" t="s">
-        <v>418</v>
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
@@ -2996,18 +3002,18 @@
         <v>36</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F20" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="11"/>
       <c r="J20" s="39" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -3448,18 +3454,18 @@
         <v>36</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F31" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="1"/>
       <c r="J31" s="39" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -3488,18 +3494,18 @@
         <v>36</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F32" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="1"/>
       <c r="J32" s="39" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
@@ -3521,7 +3527,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>35</v>
@@ -3533,15 +3539,15 @@
         <v>52</v>
       </c>
       <c r="F33" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="G33" s="41" t="s">
         <v>468</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>469</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -3932,20 +3938,20 @@
         <v>141</v>
       </c>
       <c r="E43" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="H43" s="46" t="s">
         <v>482</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="H43" s="46" t="s">
-        <v>483</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
@@ -4140,18 +4146,18 @@
         <v>141</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F48" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="11"/>
       <c r="J48" s="39" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K48" s="11"/>
       <c r="L48" s="11">
@@ -4511,7 +4517,7 @@
         <v>179</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>167</v>
@@ -4520,20 +4526,20 @@
         <v>168</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F57" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I57" s="11"/>
       <c r="J57" s="39" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
@@ -4603,7 +4609,7 @@
         <v>37</v>
       </c>
       <c r="F59" s="48" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -4644,10 +4650,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H60" s="39" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
@@ -4680,16 +4686,16 @@
         <v>183</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F61" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G61" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="H61" s="39" t="s">
         <v>422</v>
-      </c>
-      <c r="H61" s="39" t="s">
-        <v>423</v>
       </c>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
@@ -4914,20 +4920,20 @@
         <v>196</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F67" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I67" s="11"/>
       <c r="J67" s="39" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
@@ -5364,7 +5370,7 @@
       <c r="A78" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B78" s="15"/>
+      <c r="B78" s="49"/>
       <c r="C78" s="7" t="s">
         <v>237</v>
       </c>
@@ -5372,15 +5378,21 @@
         <v>238</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="F78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
+        <v>471</v>
+      </c>
+      <c r="F78" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>511</v>
+      </c>
       <c r="I78" s="7"/>
-      <c r="J78" s="7"/>
+      <c r="J78" s="39" t="s">
+        <v>470</v>
+      </c>
       <c r="K78" s="7"/>
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
@@ -5398,7 +5410,7 @@
     </row>
     <row r="79" spans="1:25" ht="100.05" customHeight="1">
       <c r="A79" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="7" t="s">
@@ -5414,12 +5426,12 @@
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
@@ -5438,7 +5450,7 @@
     </row>
     <row r="80" spans="1:25" ht="100.05" customHeight="1">
       <c r="A80" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="7" t="s">
@@ -5454,12 +5466,12 @@
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K80" s="7"/>
       <c r="L80" s="7"/>
@@ -5478,7 +5490,7 @@
     </row>
     <row r="81" spans="1:24" ht="100.05" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="7" t="s">
@@ -5494,12 +5506,12 @@
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K81" s="7"/>
       <c r="L81" s="7"/>
@@ -5518,7 +5530,7 @@
     </row>
     <row r="82" spans="1:24" ht="100.05" customHeight="1">
       <c r="A82" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="7" t="s">
@@ -5534,12 +5546,12 @@
         <v>0</v>
       </c>
       <c r="G82" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K82" s="7"/>
       <c r="L82" s="7"/>
@@ -5558,10 +5570,10 @@
     </row>
     <row r="83" spans="1:24" ht="100.05" customHeight="1">
       <c r="A83" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>237</v>
@@ -5570,20 +5582,20 @@
         <v>238</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F83" s="44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="39" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K83" s="7"/>
       <c r="L83" s="7"/>
@@ -5602,10 +5614,10 @@
     </row>
     <row r="84" spans="1:24" customFormat="1" ht="145.19999999999999">
       <c r="A84" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>237</v>
@@ -5614,20 +5626,20 @@
         <v>238</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F84" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I84" s="11"/>
       <c r="J84" s="39" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K84" s="11"/>
       <c r="L84" s="11"/>
@@ -5646,7 +5658,7 @@
     </row>
     <row r="85" spans="1:24" customFormat="1" ht="52.8">
       <c r="A85" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B85" s="10" t="s">
         <v>34</v>
@@ -5684,7 +5696,7 @@
     </row>
     <row r="86" spans="1:24" customFormat="1" ht="39.6">
       <c r="A86" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B86" s="10" t="s">
         <v>34</v>
@@ -5722,7 +5734,7 @@
     </row>
     <row r="87" spans="1:24" customFormat="1" ht="26.4">
       <c r="A87" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B87" s="10" t="s">
         <v>34</v>
@@ -5760,10 +5772,10 @@
     </row>
     <row r="88" spans="1:24" customFormat="1" ht="52.8">
       <c r="A88" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C88" s="11" t="s">
         <v>237</v>
@@ -5778,12 +5790,12 @@
         <v>0</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="11"/>
       <c r="J88" s="39" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K88" s="11"/>
       <c r="L88" s="11"/>
@@ -5802,7 +5814,7 @@
     </row>
     <row r="89" spans="1:24" customFormat="1" ht="105.6">
       <c r="A89" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="11" t="s">
@@ -5812,20 +5824,20 @@
         <v>238</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F89" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K89" s="11"/>
       <c r="L89" s="11"/>
@@ -5844,7 +5856,7 @@
     </row>
     <row r="90" spans="1:24" customFormat="1" ht="52.8">
       <c r="A90" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="11" t="s">
@@ -5854,20 +5866,20 @@
         <v>238</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F90" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G90" s="41" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I90" s="11"/>
       <c r="J90" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K90" s="11"/>
       <c r="L90" s="11"/>
@@ -5886,7 +5898,7 @@
     </row>
     <row r="91" spans="1:24" customFormat="1" ht="52.8">
       <c r="A91" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="11" t="s">
@@ -5896,20 +5908,20 @@
         <v>238</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F91" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G91" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="H91" s="7" t="s">
         <v>476</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>477</v>
       </c>
       <c r="I91" s="11"/>
       <c r="J91" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K91" s="11"/>
       <c r="L91" s="11"/>
@@ -5928,14 +5940,14 @@
     </row>
     <row r="92" spans="1:24" ht="100.05" customHeight="1">
       <c r="A92" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>115</v>
@@ -5944,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
@@ -5966,7 +5978,7 @@
     </row>
     <row r="93" spans="1:24" customFormat="1" ht="39.6">
       <c r="A93" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>34</v>
@@ -5975,7 +5987,7 @@
         <v>237</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>37</v>
@@ -6004,14 +6016,14 @@
     </row>
     <row r="94" spans="1:24" ht="100.05" customHeight="1">
       <c r="A94" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>115</v>
@@ -6020,12 +6032,12 @@
         <v>1</v>
       </c>
       <c r="G94" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K94" s="7"/>
       <c r="L94" s="7"/>
@@ -6044,23 +6056,23 @@
     </row>
     <row r="95" spans="1:24" ht="100.05" customHeight="1">
       <c r="A95" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F95" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G95" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
@@ -6082,23 +6094,23 @@
     </row>
     <row r="96" spans="1:24" ht="100.05" customHeight="1">
       <c r="A96" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F96" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G96" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
@@ -6120,23 +6132,23 @@
     </row>
     <row r="97" spans="1:25" ht="100.05" customHeight="1">
       <c r="A97" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="7" t="s">
         <v>237</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F97" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G97" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
@@ -6158,7 +6170,7 @@
     </row>
     <row r="98" spans="1:25" customFormat="1" ht="26.4">
       <c r="A98" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>34</v>
@@ -6167,7 +6179,7 @@
         <v>237</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>37</v>
@@ -6196,7 +6208,7 @@
     </row>
     <row r="99" spans="1:25" customFormat="1" ht="26.4">
       <c r="A99" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B99" s="10" t="s">
         <v>34</v>
@@ -6205,7 +6217,7 @@
         <v>237</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>37</v>
@@ -6234,7 +6246,7 @@
     </row>
     <row r="100" spans="1:25" customFormat="1" ht="66">
       <c r="A100" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>34</v>
@@ -6243,7 +6255,7 @@
         <v>237</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>37</v>
@@ -6252,14 +6264,14 @@
         <v>0</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I100" s="11"/>
       <c r="J100" s="39" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K100" s="11"/>
       <c r="L100" s="11"/>
@@ -6278,28 +6290,28 @@
     </row>
     <row r="101" spans="1:25" customFormat="1" ht="52.8">
       <c r="A101" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C101" s="11" t="s">
         <v>237</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F101" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G101" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="H101" s="39" t="s">
         <v>445</v>
-      </c>
-      <c r="H101" s="39" t="s">
-        <v>446</v>
       </c>
       <c r="I101" s="11"/>
       <c r="J101" s="11"/>
@@ -6320,14 +6332,14 @@
     </row>
     <row r="102" spans="1:25" ht="100.05" customHeight="1">
       <c r="A102" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B102" s="13"/>
       <c r="C102" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D102" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="D102" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>169</v>
@@ -6336,10 +6348,10 @@
         <v>1</v>
       </c>
       <c r="G102" t="s">
+        <v>281</v>
+      </c>
+      <c r="H102" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>283</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
@@ -6373,28 +6385,28 @@
     </row>
     <row r="103" spans="1:25" ht="100.05" customHeight="1">
       <c r="A103" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B103" s="13"/>
       <c r="C103" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D103" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="E103" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F103" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G103" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K103" s="7"/>
       <c r="L103" s="7"/>
@@ -6411,33 +6423,33 @@
       <c r="W103" s="7"/>
       <c r="X103" s="7"/>
       <c r="Y103" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:25" ht="100.05" customHeight="1">
       <c r="A104" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D104" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D104" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="E104" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F104" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G104" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K104" s="7"/>
       <c r="L104" s="7"/>
@@ -6456,23 +6468,23 @@
     </row>
     <row r="105" spans="1:25" ht="100.05" customHeight="1">
       <c r="A105" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D105" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="E105" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F105" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G105" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
@@ -6494,28 +6506,28 @@
     </row>
     <row r="106" spans="1:25" ht="100.05" customHeight="1">
       <c r="A106" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D106" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D106" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="E106" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F106" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K106" s="7"/>
       <c r="L106" s="7"/>
@@ -6534,30 +6546,30 @@
     </row>
     <row r="107" spans="1:25" ht="100.05" customHeight="1">
       <c r="A107" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B107" s="42" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C107" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D107" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D107" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="E107" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F107" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K107" s="7"/>
       <c r="L107" s="7"/>
@@ -6576,26 +6588,26 @@
     </row>
     <row r="108" spans="1:25" ht="100.05" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B108" s="28"/>
       <c r="C108" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D108" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D108" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="E108" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F108" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G108" t="s">
+        <v>451</v>
+      </c>
+      <c r="H108" s="39" t="s">
         <v>452</v>
-      </c>
-      <c r="H108" s="39" t="s">
-        <v>453</v>
       </c>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
@@ -6606,7 +6618,7 @@
       <c r="O108" s="7"/>
       <c r="P108" s="7"/>
       <c r="Q108" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R108" s="7"/>
       <c r="S108" s="7"/>
@@ -6618,7 +6630,7 @@
     </row>
     <row r="109" spans="1:25" ht="100.05" customHeight="1">
       <c r="A109" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B109" s="15"/>
       <c r="C109" s="7"/>
@@ -6648,26 +6660,26 @@
     </row>
     <row r="110" spans="1:25" ht="100.05" customHeight="1">
       <c r="A110" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D110" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E110" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="E110" s="7" t="s">
-        <v>302</v>
       </c>
       <c r="F110" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G110" t="s">
+        <v>302</v>
+      </c>
+      <c r="H110" s="7" t="s">
         <v>303</v>
-      </c>
-      <c r="H110" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
@@ -6688,14 +6700,14 @@
     </row>
     <row r="111" spans="1:25" ht="100.05" customHeight="1">
       <c r="A111" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B111" s="13"/>
       <c r="C111" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>31</v>
@@ -6704,14 +6716,14 @@
         <v>1</v>
       </c>
       <c r="G111" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H111" s="25" t="s">
         <v>306</v>
-      </c>
-      <c r="H111" s="25" t="s">
-        <v>307</v>
       </c>
       <c r="I111" s="7"/>
       <c r="J111" s="20" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K111" s="7"/>
       <c r="L111" s="7"/>
@@ -6728,37 +6740,37 @@
       <c r="W111" s="7"/>
       <c r="X111" s="7"/>
       <c r="Y111" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="112" spans="1:25" customFormat="1" ht="145.19999999999999">
       <c r="A112" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F112" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I112" s="11"/>
       <c r="J112" s="39" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K112" s="11"/>
       <c r="L112" s="11"/>
@@ -6777,32 +6789,32 @@
     </row>
     <row r="113" spans="1:25" customFormat="1" ht="145.19999999999999">
       <c r="A113" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F113" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I113" s="11"/>
       <c r="J113" s="39" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K113" s="11"/>
       <c r="L113" s="11"/>
@@ -6821,16 +6833,16 @@
     </row>
     <row r="114" spans="1:25" customFormat="1" ht="39.6">
       <c r="A114" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E114" s="11" t="s">
         <v>52</v>
@@ -6839,12 +6851,12 @@
         <v>1</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H114" s="7"/>
       <c r="I114" s="11"/>
       <c r="J114" s="18" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K114" s="11"/>
       <c r="L114" s="11"/>
@@ -6863,28 +6875,28 @@
     </row>
     <row r="115" spans="1:25" customFormat="1" ht="52.8">
       <c r="A115" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B115" s="6"/>
       <c r="C115" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F115" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H115" s="7"/>
       <c r="I115" s="11"/>
       <c r="J115" s="39" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K115" s="11"/>
       <c r="L115" s="11"/>
@@ -6903,30 +6915,30 @@
     </row>
     <row r="116" spans="1:25" ht="115.2" customHeight="1">
       <c r="A116" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B116" s="47"/>
       <c r="C116" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G116" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I116" s="7"/>
       <c r="J116" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K116" s="7"/>
       <c r="L116" s="7"/>
@@ -6945,16 +6957,16 @@
     </row>
     <row r="117" spans="1:25" customFormat="1" ht="52.8">
       <c r="A117" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B117" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E117" s="11" t="s">
         <v>37</v>
@@ -6983,16 +6995,16 @@
     </row>
     <row r="118" spans="1:25" customFormat="1" ht="52.8">
       <c r="A118" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B118" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D118" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>37</v>
@@ -7021,16 +7033,16 @@
     </row>
     <row r="119" spans="1:25" customFormat="1" ht="66">
       <c r="A119" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B119" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E119" s="11" t="s">
         <v>37</v>
@@ -7059,16 +7071,16 @@
     </row>
     <row r="120" spans="1:25" customFormat="1" ht="52.8">
       <c r="A120" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B120" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>37</v>
@@ -7097,28 +7109,28 @@
     </row>
     <row r="121" spans="1:25" ht="100.05" customHeight="1">
       <c r="A121" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B121" s="13"/>
       <c r="C121" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F121" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G121" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K121" s="7"/>
       <c r="L121" s="7"/>
@@ -7135,21 +7147,21 @@
       <c r="W121" s="7"/>
       <c r="X121" s="7"/>
       <c r="Y121" s="36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" spans="1:25" customFormat="1" ht="26.4">
       <c r="A122" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B122" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E122" s="11" t="s">
         <v>37</v>
@@ -7178,16 +7190,16 @@
     </row>
     <row r="123" spans="1:25" customFormat="1" ht="13.2">
       <c r="A123" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B123" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E123" s="11" t="s">
         <v>37</v>
@@ -7216,16 +7228,16 @@
     </row>
     <row r="124" spans="1:25" customFormat="1" ht="26.4">
       <c r="A124" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B124" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E124" s="11" t="s">
         <v>37</v>
@@ -7254,16 +7266,16 @@
     </row>
     <row r="125" spans="1:25" customFormat="1" ht="13.2">
       <c r="A125" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B125" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E125" s="11" t="s">
         <v>37</v>
@@ -7292,30 +7304,30 @@
     </row>
     <row r="126" spans="1:25" customFormat="1" ht="66">
       <c r="A126" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F126" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H126" s="1"/>
       <c r="I126" s="11"/>
       <c r="J126" s="39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K126" s="11"/>
       <c r="L126" s="11"/>
@@ -7334,16 +7346,16 @@
     </row>
     <row r="127" spans="1:25" customFormat="1" ht="13.2">
       <c r="A127" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B127" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C127" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E127" s="11" t="s">
         <v>37</v>
@@ -7372,16 +7384,16 @@
     </row>
     <row r="128" spans="1:25" customFormat="1" ht="26.4">
       <c r="A128" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B128" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E128" s="11" t="s">
         <v>37</v>
@@ -7410,16 +7422,16 @@
     </row>
     <row r="129" spans="1:25" customFormat="1" ht="13.2">
       <c r="A129" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B129" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C129" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E129" s="11" t="s">
         <v>37</v>
@@ -7448,26 +7460,26 @@
     </row>
     <row r="130" spans="1:25" ht="100.05" customHeight="1">
       <c r="A130" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F130" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G130" t="s">
+        <v>334</v>
+      </c>
+      <c r="H130" s="37" t="s">
         <v>335</v>
-      </c>
-      <c r="H130" s="37" t="s">
-        <v>336</v>
       </c>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
@@ -7488,23 +7500,23 @@
     </row>
     <row r="131" spans="1:25" ht="100.05" customHeight="1">
       <c r="A131" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D131" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="E131" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="F131" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G131" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
@@ -7526,30 +7538,30 @@
     </row>
     <row r="132" spans="1:25" customFormat="1" ht="105.6">
       <c r="A132" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B132" s="6"/>
       <c r="C132" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D132" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F132" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G132" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="H132" s="7" t="s">
         <v>485</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>486</v>
       </c>
       <c r="I132" s="11"/>
       <c r="J132" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K132" s="11"/>
       <c r="L132" s="11"/>
@@ -7568,30 +7580,30 @@
     </row>
     <row r="133" spans="1:25" customFormat="1" ht="79.2">
       <c r="A133" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B133" s="6"/>
       <c r="C133" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F133" s="11" t="b">
         <v>0</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I133" s="11"/>
       <c r="J133" s="39" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K133" s="11"/>
       <c r="L133" s="11"/>
@@ -7610,23 +7622,23 @@
     </row>
     <row r="134" spans="1:25" ht="100.05" customHeight="1">
       <c r="A134" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B134" s="13"/>
       <c r="C134" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D134" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F134" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G134" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
@@ -7646,28 +7658,28 @@
       <c r="W134" s="7"/>
       <c r="X134" s="7"/>
       <c r="Y134" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="135" spans="1:25" ht="100.05" customHeight="1">
       <c r="A135" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B135" s="13"/>
       <c r="C135" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D135" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="E135" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="E135" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="F135" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G135" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
@@ -7687,28 +7699,28 @@
       <c r="W135" s="7"/>
       <c r="X135" s="7"/>
       <c r="Y135" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="136" spans="1:25" ht="100.05" customHeight="1">
       <c r="A136" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B136" s="13"/>
       <c r="C136" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D136" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="E136" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="E136" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="F136" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G136" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
@@ -7728,19 +7740,19 @@
       <c r="W136" s="7"/>
       <c r="X136" s="7"/>
       <c r="Y136" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:25" ht="100.05" customHeight="1">
       <c r="A137" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B137" s="13"/>
       <c r="C137" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>52</v>
@@ -7749,12 +7761,12 @@
         <v>1</v>
       </c>
       <c r="G137" s="41" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K137" s="7"/>
       <c r="L137" s="7"/>
@@ -7778,16 +7790,16 @@
     </row>
     <row r="138" spans="1:25" customFormat="1" ht="52.8">
       <c r="A138" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D138" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E138" s="11" t="s">
         <v>52</v>
@@ -7796,12 +7808,12 @@
         <v>1</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="11"/>
       <c r="J138" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K138" s="11"/>
       <c r="L138" s="11"/>
@@ -7820,14 +7832,14 @@
     </row>
     <row r="139" spans="1:25" ht="100.05" customHeight="1">
       <c r="A139" s="17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B139" s="13"/>
       <c r="C139" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D139" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E139" s="7" t="s">
         <v>115</v>
@@ -7836,10 +7848,10 @@
         <v>0</v>
       </c>
       <c r="G139" s="41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H139" s="39" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -7860,14 +7872,14 @@
     </row>
     <row r="140" spans="1:25" ht="100.05" customHeight="1">
       <c r="A140" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B140" s="42"/>
       <c r="C140" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>115</v>
@@ -7876,12 +7888,12 @@
         <v>0</v>
       </c>
       <c r="G140" s="41" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
       <c r="J140" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K140" s="7"/>
       <c r="L140" s="7"/>
@@ -7897,33 +7909,33 @@
       <c r="V140" s="7"/>
       <c r="W140" s="7"/>
       <c r="X140" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="141" spans="1:25" ht="100.05" customHeight="1">
       <c r="A141" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B141" s="40"/>
       <c r="C141" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D141" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F141" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K141" s="7"/>
       <c r="L141" s="7"/>
@@ -7942,14 +7954,14 @@
     </row>
     <row r="142" spans="1:25" ht="100.05" customHeight="1">
       <c r="A142" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B142" s="42"/>
       <c r="C142" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E142" s="11" t="s">
         <v>52</v>
@@ -7958,12 +7970,12 @@
         <v>1</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
       <c r="J142" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K142" s="7"/>
       <c r="L142" s="7"/>
@@ -7979,28 +7991,28 @@
       <c r="V142" s="7"/>
       <c r="W142" s="7"/>
       <c r="X142" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="143" spans="1:25" ht="100.05" customHeight="1">
       <c r="A143" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B143" s="8"/>
       <c r="C143" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F143" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G143" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
@@ -8019,33 +8031,33 @@
       <c r="V143" s="7"/>
       <c r="W143" s="7"/>
       <c r="X143" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="144" spans="1:25" ht="100.05" customHeight="1">
       <c r="A144" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B144" s="8"/>
       <c r="C144" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F144" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G144" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
       <c r="J144" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K144" s="7"/>
       <c r="L144" s="7"/>
@@ -8061,28 +8073,28 @@
       <c r="V144" s="7"/>
       <c r="W144" s="7"/>
       <c r="X144" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="145" spans="1:25" ht="100.05" customHeight="1">
       <c r="A145" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B145" s="8"/>
       <c r="C145" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F145" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G145" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -8101,21 +8113,21 @@
       <c r="V145" s="7"/>
       <c r="W145" s="7"/>
       <c r="X145" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="146" spans="1:25" customFormat="1" ht="26.4">
       <c r="A146" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D146" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E146" s="11" t="s">
         <v>115</v>
@@ -8124,10 +8136,10 @@
         <v>0</v>
       </c>
       <c r="G146" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H146" s="39" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I146" s="11"/>
       <c r="J146" s="11"/>
@@ -8148,14 +8160,14 @@
     </row>
     <row r="147" spans="1:25" ht="100.05" customHeight="1">
       <c r="A147" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B147" s="8"/>
       <c r="C147" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>190</v>
@@ -8164,7 +8176,7 @@
         <v>0</v>
       </c>
       <c r="G147" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
@@ -8186,16 +8198,16 @@
     </row>
     <row r="148" spans="1:25" customFormat="1" ht="39.6">
       <c r="A148" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D148" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E148" s="11" t="s">
         <v>48</v>
@@ -8204,10 +8216,10 @@
         <v>0</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H148" s="39" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I148" s="11"/>
       <c r="J148" s="11"/>
@@ -8225,19 +8237,19 @@
       <c r="V148" s="11"/>
       <c r="W148" s="11"/>
       <c r="X148" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="149" spans="1:25" ht="100.05" customHeight="1">
       <c r="A149" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B149" s="8"/>
       <c r="C149" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E149" s="7" t="s">
         <v>52</v>
@@ -8246,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="G149" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
@@ -8267,28 +8279,28 @@
       <c r="V149" s="7"/>
       <c r="W149" s="7"/>
       <c r="X149" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="150" spans="1:25" ht="100.05" customHeight="1">
       <c r="A150" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B150" s="8"/>
       <c r="C150" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="D150" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="D150" s="7" t="s">
+      <c r="E150" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="E150" s="7" t="s">
-        <v>378</v>
       </c>
       <c r="F150" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G150" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
@@ -8310,30 +8322,30 @@
     </row>
     <row r="151" spans="1:25" ht="100.05" customHeight="1">
       <c r="A151" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B151" s="13"/>
       <c r="C151" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D151" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="D151" s="7" t="s">
-        <v>382</v>
-      </c>
       <c r="E151" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F151" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G151" s="41" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I151" s="7"/>
       <c r="J151" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K151" s="7"/>
       <c r="L151" s="7"/>
@@ -8350,21 +8362,21 @@
       <c r="W151" s="7"/>
       <c r="X151" s="7"/>
       <c r="Y151" s="38" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="152" spans="1:25" ht="100.05" customHeight="1">
       <c r="A152" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B152" s="50" t="s">
         <v>385</v>
       </c>
-      <c r="B152" s="49" t="s">
-        <v>386</v>
-      </c>
       <c r="C152" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D152" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="D152" s="7" t="s">
-        <v>382</v>
       </c>
       <c r="E152" s="7" t="s">
         <v>190</v>
@@ -8373,7 +8385,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
@@ -8395,14 +8407,14 @@
     </row>
     <row r="153" spans="1:25" ht="100.05" customHeight="1">
       <c r="A153" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="B153" s="49"/>
+        <v>386</v>
+      </c>
+      <c r="B153" s="50"/>
       <c r="C153" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D153" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="D153" s="7" t="s">
-        <v>382</v>
       </c>
       <c r="E153" s="7" t="s">
         <v>190</v>
@@ -8411,7 +8423,7 @@
         <v>0</v>
       </c>
       <c r="G153" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
@@ -8433,14 +8445,14 @@
     </row>
     <row r="154" spans="1:25" ht="100.05" customHeight="1">
       <c r="A154" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="B154" s="49"/>
+        <v>387</v>
+      </c>
+      <c r="B154" s="50"/>
       <c r="C154" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D154" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>382</v>
       </c>
       <c r="E154" s="7" t="s">
         <v>190</v>
@@ -8469,14 +8481,14 @@
     </row>
     <row r="155" spans="1:25" ht="100.05" customHeight="1">
       <c r="A155" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="B155" s="49"/>
+        <v>388</v>
+      </c>
+      <c r="B155" s="50"/>
       <c r="C155" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D155" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="D155" s="7" t="s">
-        <v>382</v>
       </c>
       <c r="E155" s="7" t="s">
         <v>190</v>
@@ -8505,28 +8517,28 @@
     </row>
     <row r="156" spans="1:25" ht="100.05" customHeight="1">
       <c r="A156" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="B156" s="51"/>
+      <c r="C156" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D156" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="B156" s="50"/>
-      <c r="C156" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="D156" s="7" t="s">
+      <c r="E156" s="7" t="s">
         <v>391</v>
-      </c>
-      <c r="E156" s="7" t="s">
-        <v>392</v>
       </c>
       <c r="F156" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G156" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H156" s="7"/>
       <c r="I156" s="7"/>
       <c r="J156" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K156" s="7"/>
       <c r="L156" s="7"/>
@@ -8545,23 +8557,23 @@
     </row>
     <row r="157" spans="1:25" ht="100.05" customHeight="1">
       <c r="A157" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B157" s="50"/>
+        <v>394</v>
+      </c>
+      <c r="B157" s="51"/>
       <c r="C157" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D157" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="E157" s="7" t="s">
         <v>391</v>
-      </c>
-      <c r="E157" s="7" t="s">
-        <v>392</v>
       </c>
       <c r="F157" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G157" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
@@ -8583,14 +8595,14 @@
     </row>
     <row r="158" spans="1:25" ht="100.05" customHeight="1">
       <c r="A158" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B158" s="49"/>
+        <v>394</v>
+      </c>
+      <c r="B158" s="50"/>
       <c r="C158" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D158" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E158" s="7" t="s">
         <v>190</v>
@@ -8599,7 +8611,7 @@
         <v>0</v>
       </c>
       <c r="G158" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H158" s="7"/>
       <c r="I158" s="7"/>
@@ -8621,14 +8633,14 @@
     </row>
     <row r="159" spans="1:25" customFormat="1" ht="26.4">
       <c r="A159" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="B159" s="50"/>
+        <v>395</v>
+      </c>
+      <c r="B159" s="51"/>
       <c r="C159" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E159" s="11" t="s">
         <v>37</v>
@@ -8637,7 +8649,7 @@
         <v>0</v>
       </c>
       <c r="G159" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H159" s="7"/>
       <c r="I159" s="11"/>
@@ -8659,14 +8671,14 @@
     </row>
     <row r="160" spans="1:25" ht="100.05" customHeight="1">
       <c r="A160" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="B160" s="49"/>
+        <v>396</v>
+      </c>
+      <c r="B160" s="50"/>
       <c r="C160" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E160" s="7" t="s">
         <v>190</v>
@@ -8675,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="G160" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
@@ -8697,16 +8709,16 @@
     </row>
     <row r="161" spans="1:24" customFormat="1" ht="13.2">
       <c r="A161" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B161" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E161" s="11" t="s">
         <v>37</v>
@@ -8735,28 +8747,28 @@
     </row>
     <row r="162" spans="1:24" ht="100.05" customHeight="1">
       <c r="A162" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B162" s="8"/>
       <c r="C162" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D162" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="E162" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="E162" s="7" t="s">
-        <v>401</v>
       </c>
       <c r="F162" s="7" t="b">
         <v>1</v>
       </c>
       <c r="G162" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H162" s="7"/>
       <c r="I162" s="7"/>
       <c r="J162" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K162" s="7"/>
       <c r="L162" s="7"/>
@@ -8770,23 +8782,23 @@
       <c r="T162" s="7"/>
       <c r="U162" s="7"/>
       <c r="V162" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="W162" s="7"/>
       <c r="X162" s="7"/>
     </row>
     <row r="163" spans="1:24" customFormat="1" ht="26.4">
       <c r="A163" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B163" s="15" t="s">
         <v>34</v>
       </c>
       <c r="C163" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E163" s="11" t="s">
         <v>37</v>
@@ -34161,6 +34173,7 @@
     <hyperlink ref="J112" r:id="rId94" xr:uid="{19C0F1DB-8225-41BB-A3C4-07150C53A371}"/>
     <hyperlink ref="J116" r:id="rId95" xr:uid="{F26C5D2D-560A-47D8-A8B6-BDA23E99E1F0}"/>
     <hyperlink ref="H9" r:id="rId96" xr:uid="{C8866DBC-A5B7-4478-BAF6-254943B6CEC6}"/>
+    <hyperlink ref="J78" r:id="rId97" xr:uid="{01FA22C8-1DB6-4FF8-B54E-6431AAC109A1}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="120" orientation="portrait"/>

</xml_diff>

<commit_message>
change the top row of 2 excel files
</commit_message>
<xml_diff>
--- a/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
+++ b/UNDP Digital Assessment Data Framework Filename Matching V7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stan Smith\Documents\GIT\UNDP\digital-readiness-assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C120DC7-14F4-4D85-A3F7-395462EF01B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030A1E49-5163-45EC-9AD2-DDE15F43A953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3167,10 +3167,10 @@
   <dimension ref="A1:AD1132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C157" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C152" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G171" sqref="G171"/>
+      <selection pane="bottomRight" activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>